<commit_message>
Republication complète site (Excel fermés)
</commit_message>
<xml_diff>
--- a/prix/geka.xlsx
+++ b/prix/geka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\raccords-plomberie\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7850F73-018C-4006-9C89-47851599374C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB63C03A-4E57-41F6-AB65-F1B1A9E3B810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E54DEEA7-0B41-4DCD-A45B-352BD142BB27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>43040909</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>38</t>
+  </si>
+  <si>
+    <t>geka/rac-geka-F.png</t>
+  </si>
+  <si>
+    <t>geka/rac-geka-M.png</t>
+  </si>
+  <si>
+    <t>geka/rac-geka-T.png</t>
   </si>
 </sst>
 </file>
@@ -600,12 +609,12 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" activeCellId="1" sqref="G1:G1048576 F1:F1048576"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="8"/>
+    <col min="1" max="1" width="17.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.21875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" style="7"/>
     <col min="4" max="5" width="11.5546875" style="8"/>
@@ -645,6 +654,9 @@
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -659,6 +671,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
@@ -673,6 +688,9 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
@@ -687,6 +705,9 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
@@ -701,6 +722,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
@@ -715,6 +739,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -729,6 +756,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -743,6 +773,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
@@ -757,6 +790,9 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
@@ -771,6 +807,9 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
@@ -785,6 +824,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="B12" s="7" t="s">
         <v>21</v>
       </c>
@@ -824,6 +866,9 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="B15" s="7" t="s">
         <v>27</v>
       </c>
@@ -838,6 +883,9 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="B16" s="7" t="s">
         <v>29</v>
       </c>
@@ -851,7 +899,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
@@ -865,7 +916,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
@@ -879,7 +933,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="B19" s="7" t="s">
         <v>35</v>
       </c>

</xml_diff>